<commit_message>
Continued on the Excel sheet
</commit_message>
<xml_diff>
--- a/Oracle/Assignment 4/Ammar/Group_11_Assignment_4.xlsx
+++ b/Oracle/Assignment 4/Ammar/Group_11_Assignment_4.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F451A62F-823B-437D-A95A-6EE0A685F378}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80E9874-7C6D-9F44-BD57-C8CF587827C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="56535" yWindow="1440" windowWidth="28800" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uprise Art" sheetId="2" r:id="rId1"/>
@@ -15,9 +15,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -156,7 +154,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;???_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;???_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -220,10 +218,10 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -240,7 +238,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -562,33 +560,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="30.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
-    <col min="5" max="5" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="20.90625" customWidth="1"/>
-    <col min="8" max="8" width="19.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.90625" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20.83203125" customWidth="1"/>
+    <col min="8" max="8" width="19.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="14" max="14" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.90625" customWidth="1"/>
-    <col min="16" max="16" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.90625" customWidth="1"/>
+    <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.83203125" customWidth="1"/>
+    <col min="16" max="16" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -635,7 +633,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -692,7 +690,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -747,7 +745,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -778,7 +776,7 @@
         <v>10</v>
       </c>
       <c r="J4">
-        <f t="shared" si="2"/>
+        <f>B4*F4*(1+E4/100)*(1+I4/100)</f>
         <v>464969.12000000005</v>
       </c>
       <c r="K4" s="11">
@@ -786,7 +784,7 @@
         <v>454.07140625000005</v>
       </c>
       <c r="L4" s="4">
-        <f t="shared" si="4"/>
+        <f>_xlfn.CEILING.MATH(B4*H4*(1+E4/100)*(1+I4/100),1)</f>
         <v>26499</v>
       </c>
       <c r="M4" s="2">
@@ -802,7 +800,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -859,7 +857,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -916,7 +914,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -970,7 +968,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1026,7 +1024,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1083,7 +1081,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1138,7 +1136,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1193,7 +1191,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1247,7 +1245,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1301,13 +1299,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="K14" s="3"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1329,7 +1327,7 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1354,7 +1352,7 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>15</v>
       </c>
@@ -1373,7 +1371,7 @@
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>16</v>
       </c>
@@ -1391,7 +1389,7 @@
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>17</v>
       </c>
@@ -1406,7 +1404,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>19</v>
       </c>
@@ -1421,31 +1419,31 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>20</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1457,12 +1455,12 @@
       </c>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1476,12 +1474,12 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1495,12 +1493,12 @@
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1514,39 +1512,39 @@
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:9" x14ac:dyDescent="0.2">
       <c r="E33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:9" x14ac:dyDescent="0.2">
       <c r="E34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="5:9" x14ac:dyDescent="0.2">
       <c r="E35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="5:9" x14ac:dyDescent="0.2">
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="5:9" x14ac:dyDescent="0.2">
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="5:9" x14ac:dyDescent="0.2">
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="5:9" x14ac:dyDescent="0.2">
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
     </row>

</xml_diff>